<commit_message>
Finished Spectra Calculation, Starting working on Summing all spectra
</commit_message>
<xml_diff>
--- a/X2110-Camera/100x/bQD705-5/all-bQD705.xlsx
+++ b/X2110-Camera/100x/bQD705-5/all-bQD705.xlsx
@@ -24,12 +24,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>centers</t>
   </si>
   <si>
     <t>sigmas</t>
+  </si>
+  <si>
+    <t>AVG</t>
+  </si>
+  <si>
+    <t>STD</t>
+  </si>
+  <si>
+    <t>Err AVG</t>
+  </si>
+  <si>
+    <t>Disper</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>ARR Width</t>
   </si>
 </sst>
 </file>
@@ -50,12 +71,24 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -85,11 +118,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,15 +439,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB7AC27-AA9D-4585-8539-343CD1E00CBF}">
-  <dimension ref="A1:C107"/>
+  <dimension ref="A1:E108"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B108" sqref="B108"/>
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,7 +455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -430,8 +465,11 @@
       <c r="C2">
         <v>23.406824537102398</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -441,8 +479,11 @@
       <c r="C3">
         <v>26.0944900476523</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -452,8 +493,11 @@
       <c r="C4">
         <v>17.744294599599471</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -463,8 +507,11 @@
       <c r="C5">
         <v>22.35568136924816</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -474,8 +521,11 @@
       <c r="C6">
         <v>25.941819904568199</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -485,8 +535,11 @@
       <c r="C7">
         <v>20.79888952661959</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -496,8 +549,11 @@
       <c r="C8">
         <v>22.168121045205091</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -507,8 +563,11 @@
       <c r="C9">
         <v>24.551321377187161</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -518,8 +577,11 @@
       <c r="C10">
         <v>25.541075553210369</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -529,8 +591,11 @@
       <c r="C11">
         <v>25.315084292976149</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -540,8 +605,11 @@
       <c r="C12">
         <v>28.458228158896301</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -551,8 +619,11 @@
       <c r="C13">
         <v>27.29443155023159</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -562,8 +633,11 @@
       <c r="C14">
         <v>30.37038049601648</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -573,8 +647,11 @@
       <c r="C15">
         <v>27.697149747250801</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -584,8 +661,11 @@
       <c r="C16">
         <v>24.403385555383888</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -595,8 +675,11 @@
       <c r="C17">
         <v>25.4409830567207</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -606,8 +689,11 @@
       <c r="C18">
         <v>37.774688734495207</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -617,8 +703,11 @@
       <c r="C19">
         <v>23.40506115864267</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -628,8 +717,11 @@
       <c r="C20">
         <v>31.312570995448649</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -639,8 +731,11 @@
       <c r="C21">
         <v>26.309745363463328</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -650,8 +745,11 @@
       <c r="C22">
         <v>28.5204994378085</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -661,8 +759,11 @@
       <c r="C23">
         <v>24.415995119044041</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>0</v>
       </c>
@@ -672,8 +773,11 @@
       <c r="C24">
         <v>21.375400675336</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1</v>
       </c>
@@ -683,8 +787,11 @@
       <c r="C25">
         <v>21.895706805975401</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2</v>
       </c>
@@ -694,8 +801,11 @@
       <c r="C26">
         <v>24.220436761011111</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>3</v>
       </c>
@@ -705,8 +815,11 @@
       <c r="C27">
         <v>23.159011576772759</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>4</v>
       </c>
@@ -716,8 +829,11 @@
       <c r="C28">
         <v>27.811392286704681</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>5</v>
       </c>
@@ -727,8 +843,11 @@
       <c r="C29">
         <v>21.746860330349801</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>6</v>
       </c>
@@ -738,8 +857,11 @@
       <c r="C30">
         <v>23.855169836082151</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>7</v>
       </c>
@@ -749,8 +871,11 @@
       <c r="C31">
         <v>23.12596460143007</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>8</v>
       </c>
@@ -760,8 +885,11 @@
       <c r="C32">
         <v>20.552535249569871</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>9</v>
       </c>
@@ -771,8 +899,11 @@
       <c r="C33">
         <v>22.222848634114619</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>10</v>
       </c>
@@ -782,8 +913,11 @@
       <c r="C34">
         <v>27.091781312322759</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>11</v>
       </c>
@@ -793,8 +927,11 @@
       <c r="C35">
         <v>22.423451222393179</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>12</v>
       </c>
@@ -804,8 +941,11 @@
       <c r="C36">
         <v>31.16958272211718</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>13</v>
       </c>
@@ -815,8 +955,11 @@
       <c r="C37">
         <v>25.22173249756824</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>14</v>
       </c>
@@ -826,8 +969,11 @@
       <c r="C38">
         <v>29.138320371860129</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>15</v>
       </c>
@@ -837,8 +983,11 @@
       <c r="C39">
         <v>32.696296593973507</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>16</v>
       </c>
@@ -848,8 +997,11 @@
       <c r="C40">
         <v>23.673589750161241</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>17</v>
       </c>
@@ -859,8 +1011,11 @@
       <c r="C41">
         <v>24.838484148500971</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>18</v>
       </c>
@@ -870,8 +1025,11 @@
       <c r="C42">
         <v>28.460005122432669</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>19</v>
       </c>
@@ -881,8 +1039,11 @@
       <c r="C43">
         <v>27.364805821777001</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>20</v>
       </c>
@@ -892,8 +1053,11 @@
       <c r="C44">
         <v>22.91552358534457</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>21</v>
       </c>
@@ -903,8 +1067,11 @@
       <c r="C45">
         <v>31.886511944068761</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>22</v>
       </c>
@@ -914,8 +1081,11 @@
       <c r="C46">
         <v>25.990100384833241</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>23</v>
       </c>
@@ -925,8 +1095,11 @@
       <c r="C47">
         <v>27.549329079554429</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>24</v>
       </c>
@@ -936,8 +1109,11 @@
       <c r="C48">
         <v>27.51955157303993</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>25</v>
       </c>
@@ -947,8 +1123,11 @@
       <c r="C49">
         <v>24.09754389775911</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>0</v>
       </c>
@@ -958,8 +1137,11 @@
       <c r="C50">
         <v>44.344395652768107</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>1</v>
       </c>
@@ -969,8 +1151,11 @@
       <c r="C51">
         <v>24.059938893936341</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>2</v>
       </c>
@@ -980,8 +1165,11 @@
       <c r="C52">
         <v>47.333659179807142</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>3</v>
       </c>
@@ -991,8 +1179,11 @@
       <c r="C53">
         <v>24.267276673936891</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>4</v>
       </c>
@@ -1002,8 +1193,11 @@
       <c r="C54">
         <v>27.547396437027519</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>5</v>
       </c>
@@ -1013,8 +1207,11 @@
       <c r="C55">
         <v>25.967981216298391</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>6</v>
       </c>
@@ -1024,8 +1221,11 @@
       <c r="C56">
         <v>21.96534264267974</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>7</v>
       </c>
@@ -1035,8 +1235,11 @@
       <c r="C57">
         <v>32.013228758870937</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>8</v>
       </c>
@@ -1046,8 +1249,11 @@
       <c r="C58">
         <v>27.608768922765002</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>9</v>
       </c>
@@ -1057,8 +1263,11 @@
       <c r="C59">
         <v>26.537991300772092</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E59">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>10</v>
       </c>
@@ -1068,8 +1277,11 @@
       <c r="C60">
         <v>30.848692439579018</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E60">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>11</v>
       </c>
@@ -1079,8 +1291,11 @@
       <c r="C61">
         <v>27.763445285858712</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>12</v>
       </c>
@@ -1090,8 +1305,11 @@
       <c r="C62">
         <v>25.969008856901699</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>13</v>
       </c>
@@ -1101,8 +1319,11 @@
       <c r="C63">
         <v>30.46608780134299</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>14</v>
       </c>
@@ -1112,8 +1333,11 @@
       <c r="C64">
         <v>22.65294932568014</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>15</v>
       </c>
@@ -1123,8 +1347,11 @@
       <c r="C65">
         <v>24.954419936174261</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>16</v>
       </c>
@@ -1134,8 +1361,11 @@
       <c r="C66">
         <v>42.850230264779867</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>17</v>
       </c>
@@ -1145,8 +1375,11 @@
       <c r="C67">
         <v>44.011496865540643</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>18</v>
       </c>
@@ -1156,8 +1389,11 @@
       <c r="C68">
         <v>31.966233350920131</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E68">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>19</v>
       </c>
@@ -1167,8 +1403,11 @@
       <c r="C69">
         <v>27.611463648111489</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E69">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>20</v>
       </c>
@@ -1178,8 +1417,11 @@
       <c r="C70">
         <v>39.728106799342697</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E70">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>21</v>
       </c>
@@ -1189,8 +1431,11 @@
       <c r="C71">
         <v>29.709980251445192</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E71">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>22</v>
       </c>
@@ -1200,8 +1445,11 @@
       <c r="C72">
         <v>41.217691139704307</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E72">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>23</v>
       </c>
@@ -1211,8 +1459,11 @@
       <c r="C73">
         <v>41.049131040228879</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E73">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>24</v>
       </c>
@@ -1222,8 +1473,11 @@
       <c r="C74">
         <v>57.569074038273243</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E74">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>25</v>
       </c>
@@ -1233,8 +1487,11 @@
       <c r="C75">
         <v>31.920882989334189</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>26</v>
       </c>
@@ -1244,8 +1501,11 @@
       <c r="C76">
         <v>35.589418492611067</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E76">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>27</v>
       </c>
@@ -1255,8 +1515,11 @@
       <c r="C77">
         <v>47.308890732121448</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E77">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>28</v>
       </c>
@@ -1266,8 +1529,11 @@
       <c r="C78">
         <v>35.664540456286531</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E78">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>29</v>
       </c>
@@ -1277,8 +1543,11 @@
       <c r="C79">
         <v>44.139649314521563</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E79">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>30</v>
       </c>
@@ -1288,8 +1557,11 @@
       <c r="C80">
         <v>45.039671038462593</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E80">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>31</v>
       </c>
@@ -1299,8 +1571,11 @@
       <c r="C81">
         <v>91.771590730387686</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>0</v>
       </c>
@@ -1310,8 +1585,11 @@
       <c r="C82">
         <v>35.609122603551022</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E82">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>1</v>
       </c>
@@ -1321,8 +1599,11 @@
       <c r="C83">
         <v>49.188888270882529</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E83">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>2</v>
       </c>
@@ -1332,8 +1613,11 @@
       <c r="C84">
         <v>52.801448261401049</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E84">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>3</v>
       </c>
@@ -1343,8 +1627,11 @@
       <c r="C85">
         <v>45.871753852142312</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E85">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>4</v>
       </c>
@@ -1354,8 +1641,11 @@
       <c r="C86">
         <v>44.121997269406698</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E86">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>5</v>
       </c>
@@ -1365,8 +1655,11 @@
       <c r="C87">
         <v>41.427145074576941</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E87">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>6</v>
       </c>
@@ -1376,8 +1669,11 @@
       <c r="C88">
         <v>43.435924606752828</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E88">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>7</v>
       </c>
@@ -1387,8 +1683,11 @@
       <c r="C89">
         <v>59.866802838193827</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E89">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>8</v>
       </c>
@@ -1398,8 +1697,11 @@
       <c r="C90">
         <v>46.742207841129698</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E90">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>0</v>
       </c>
@@ -1409,8 +1711,11 @@
       <c r="C91">
         <v>24.956562987810671</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E91">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>1</v>
       </c>
@@ -1420,8 +1725,11 @@
       <c r="C92">
         <v>39.373973361256184</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E92">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>2</v>
       </c>
@@ -1431,8 +1739,11 @@
       <c r="C93">
         <v>32.473510221071002</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E93">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>3</v>
       </c>
@@ -1442,8 +1753,11 @@
       <c r="C94">
         <v>24.89029225582512</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E94">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>4</v>
       </c>
@@ -1453,8 +1767,11 @@
       <c r="C95">
         <v>45.362634935040177</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E95">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>5</v>
       </c>
@@ -1464,8 +1781,11 @@
       <c r="C96">
         <v>37.521874416536107</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E96">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>6</v>
       </c>
@@ -1475,8 +1795,11 @@
       <c r="C97">
         <v>34.480728488320182</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E97">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>7</v>
       </c>
@@ -1486,8 +1809,11 @@
       <c r="C98">
         <v>32.005341095991888</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E98">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>8</v>
       </c>
@@ -1497,8 +1823,11 @@
       <c r="C99">
         <v>35.913108800485603</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E99">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>9</v>
       </c>
@@ -1508,8 +1837,11 @@
       <c r="C100">
         <v>38.966418804701377</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E100">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>10</v>
       </c>
@@ -1519,8 +1851,14 @@
       <c r="C101">
         <v>30.72950463721013</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E101">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="B103">
         <f>AVERAGE(B2:B101)</f>
         <v>686.14019292669627</v>
@@ -1529,8 +1867,14 @@
         <f>AVERAGE(C2:C101)</f>
         <v>31.785105335105808</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="B104">
         <f>_xlfn.STDEV.P(B2:B101)</f>
         <v>5.8554390052841097</v>
@@ -1539,21 +1883,52 @@
         <f>_xlfn.STDEV.P(C2:C101)</f>
         <v>10.733411479799752</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="B105">
-        <f>B104/SQRT(100)</f>
+        <f>B104/SQRT(E101)</f>
         <v>0.58554390052841099</v>
       </c>
       <c r="C105">
-        <f>C104/SQRT(100)</f>
+        <f>C104/SQRT(E101)</f>
         <v>1.0733411479799753</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="2"/>
+      <c r="D106" s="3"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="B107">
         <f>B104/B103*100</f>
         <v>0.85338813636729705</v>
+      </c>
+      <c r="C107">
+        <f>C104/C103*100</f>
+        <v>33.768683056541526</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>